<commit_message>
funciona, genera un  PDf por por renglon, cada un con su nombre, a ver si en la siguiente version se hace un solo PDF
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DISEÑO\PROYECTOS\PERSONALES\DIPLOMATIC\CERTIFICATE_01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D5B416-82C1-417F-A612-29347853851D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C45C9E-A925-45B9-A724-140185D885CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{D6E07C82-2101-4F48-AD9D-49614C968E2E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
   <si>
     <t>Alternant matrix</t>
   </si>
@@ -254,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -262,8 +262,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -283,9 +282,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -323,7 +322,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -429,7 +428,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -571,7 +570,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -579,17 +578,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9F0046-C092-4E82-B4E8-E5335126074A}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="A11:C35"/>
+      <selection activeCell="A21" sqref="A21:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="147.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="147.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -685,6 +684,194 @@
         <v>21</v>
       </c>
       <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -699,6 +886,28 @@
     <hyperlink ref="A9" r:id="rId9" tooltip="Logical matrix" display="https://en.wikipedia.org/wiki/Logical_matrix" xr:uid="{F093AE14-496E-4CAE-B8D8-7F1E89E669C8}"/>
     <hyperlink ref="C9" r:id="rId10" location="cite_note-1" display="https://en.wikipedia.org/wiki/List_of_named_matrices - cite_note-1" xr:uid="{1562CB81-B5A9-46FA-9BF1-3672B3745C03}"/>
     <hyperlink ref="A10" r:id="rId11" tooltip="Bisymmetric matrix" display="https://en.wikipedia.org/wiki/Bisymmetric_matrix" xr:uid="{4B171FFA-2AC4-4F93-BA70-112C0448EADF}"/>
+    <hyperlink ref="A11" r:id="rId12" tooltip="Alternant matrix" display="https://en.wikipedia.org/wiki/Alternant_matrix" xr:uid="{310C3C7C-4441-42D6-9940-2B61FB54298E}"/>
+    <hyperlink ref="A12" r:id="rId13" tooltip="Alternating sign matrix" display="https://en.wikipedia.org/wiki/Alternating_sign_matrix" xr:uid="{D2612611-9E47-4980-9D89-B6FAA56B4745}"/>
+    <hyperlink ref="A13" r:id="rId14" tooltip="Anti-diagonal matrix" display="https://en.wikipedia.org/wiki/Anti-diagonal_matrix" xr:uid="{3681250C-F956-49AA-8D6A-AA0BF55E3EE0}"/>
+    <hyperlink ref="A14" r:id="rId15" tooltip="Skew-Hermitian matrix" display="https://en.wikipedia.org/wiki/Skew-Hermitian_matrix" xr:uid="{20006443-ECCA-412A-BFB0-ED681E4D98B8}"/>
+    <hyperlink ref="A15" r:id="rId16" tooltip="Skew-symmetric matrix" display="https://en.wikipedia.org/wiki/Skew-symmetric_matrix" xr:uid="{E117492E-145F-4218-A2D5-5945F037CF7F}"/>
+    <hyperlink ref="A16" r:id="rId17" tooltip="Arrowhead matrix" display="https://en.wikipedia.org/wiki/Arrowhead_matrix" xr:uid="{619AAC08-C4A9-4444-9A49-BE77C577D10B}"/>
+    <hyperlink ref="A17" r:id="rId18" tooltip="Band matrix" display="https://en.wikipedia.org/wiki/Band_matrix" xr:uid="{9B46D423-0D76-4B93-B774-536AE27008BB}"/>
+    <hyperlink ref="A18" r:id="rId19" tooltip="Bidiagonal matrix" display="https://en.wikipedia.org/wiki/Bidiagonal_matrix" xr:uid="{15A2D6F7-5889-42CB-B231-33E3D5961B46}"/>
+    <hyperlink ref="A19" r:id="rId20" tooltip="Logical matrix" display="https://en.wikipedia.org/wiki/Logical_matrix" xr:uid="{F4AE6492-B11E-4A17-9C47-8E6B1D8A6966}"/>
+    <hyperlink ref="C19" r:id="rId21" location="cite_note-1" display="https://en.wikipedia.org/wiki/List_of_named_matrices - cite_note-1" xr:uid="{29499851-EC1E-4076-AD56-192382875ACB}"/>
+    <hyperlink ref="A20" r:id="rId22" tooltip="Bisymmetric matrix" display="https://en.wikipedia.org/wiki/Bisymmetric_matrix" xr:uid="{4D8F5931-CBF5-4A80-9CA0-1568B9EE032D}"/>
+    <hyperlink ref="A21" r:id="rId23" tooltip="Alternant matrix" display="https://en.wikipedia.org/wiki/Alternant_matrix" xr:uid="{99F63946-FCEE-43E7-98C6-7C19C69D36DC}"/>
+    <hyperlink ref="A22" r:id="rId24" tooltip="Alternating sign matrix" display="https://en.wikipedia.org/wiki/Alternating_sign_matrix" xr:uid="{5446E6E4-4039-4D3E-9BCE-FA9A46FEB3EF}"/>
+    <hyperlink ref="A23" r:id="rId25" tooltip="Anti-diagonal matrix" display="https://en.wikipedia.org/wiki/Anti-diagonal_matrix" xr:uid="{3DEDDD5B-2975-47BB-B77C-476A980D2779}"/>
+    <hyperlink ref="A24" r:id="rId26" tooltip="Skew-Hermitian matrix" display="https://en.wikipedia.org/wiki/Skew-Hermitian_matrix" xr:uid="{D075EC44-3E4E-420E-8CF7-FE04ECD202B7}"/>
+    <hyperlink ref="A25" r:id="rId27" tooltip="Skew-symmetric matrix" display="https://en.wikipedia.org/wiki/Skew-symmetric_matrix" xr:uid="{6FA8E769-6D73-4D58-8717-E8FA672A2D38}"/>
+    <hyperlink ref="A26" r:id="rId28" tooltip="Arrowhead matrix" display="https://en.wikipedia.org/wiki/Arrowhead_matrix" xr:uid="{D721EB35-1DDE-4E25-9EF6-F51C8FD452EC}"/>
+    <hyperlink ref="A27" r:id="rId29" tooltip="Band matrix" display="https://en.wikipedia.org/wiki/Band_matrix" xr:uid="{0225D5D6-94CF-4BDA-AE1A-92E728D55776}"/>
+    <hyperlink ref="A28" r:id="rId30" tooltip="Bidiagonal matrix" display="https://en.wikipedia.org/wiki/Bidiagonal_matrix" xr:uid="{D635C8A2-8276-4B95-8E00-1190F2E3E687}"/>
+    <hyperlink ref="A29" r:id="rId31" tooltip="Logical matrix" display="https://en.wikipedia.org/wiki/Logical_matrix" xr:uid="{6E91D74C-0E25-4CB0-A557-72BF560F39CF}"/>
+    <hyperlink ref="C29" r:id="rId32" location="cite_note-1" display="https://en.wikipedia.org/wiki/List_of_named_matrices - cite_note-1" xr:uid="{A2D69AFA-2927-4B7C-BF05-F66C546F54F5}"/>
+    <hyperlink ref="A30" r:id="rId33" tooltip="Bisymmetric matrix" display="https://en.wikipedia.org/wiki/Bisymmetric_matrix" xr:uid="{BBD2D88C-49FC-4F90-A9B6-4B20187FC93D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>